<commit_message>
Fix typo in BOM, update project file
</commit_message>
<xml_diff>
--- a/6vleadacidsolar.xlsx
+++ b/6vleadacidsolar.xlsx
@@ -56,7 +56,7 @@
     <t>UNITED CHEMI-CON</t>
   </si>
   <si>
-    <t>EMZJ160ADR471MHA0G</t>
+    <t>EMZJ160ADA471MHA0G</t>
   </si>
   <si>
     <t>Digi-Key, Mouser</t>
@@ -449,7 +449,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>